<commit_message>
added table and token logging feature
</commit_message>
<xml_diff>
--- a/docs/Parsing table with sync.xlsx
+++ b/docs/Parsing table with sync.xlsx
@@ -1,7 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
+  <bookViews>
+    <workbookView activeTab="0"/>
+  </bookViews>
   <sheets>
     <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId3"/>
   </sheets>
@@ -145,17 +148,32 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" mc:Ignorable="x14ac">
+  <numFmts count="8">
+    <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);(&quot;$&quot;#,##0)"/>
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red](&quot;$&quot;#,##0)"/>
+    <numFmt numFmtId="7" formatCode="&quot;$&quot;#,##0.00_);(&quot;$&quot;#,##0.00)"/>
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red](&quot;$&quot;#,##0.00)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* (#,##0);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* (#,##0);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* (#,##0.00);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* (#,##0.00);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
   <fonts count="3">
     <font>
-      <sz val="10.0"/>
+      <name val="Arial"/>
       <color rgb="FF000000"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <color rgb="FF000000"/>
+      <sz val="12"/>
+    </font>
+    <font>
       <name val="Arial"/>
-    </font>
-    <font/>
-    <font>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <sz val="12"/>
     </font>
   </fonts>
   <fills count="3">
@@ -176,21 +194,17 @@
     <border/>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
 </styleSheet>
@@ -201,17 +215,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection pane="topLeft" activeCell="K14" sqref="K14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="14.43" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="7.43"/>
-    <col customWidth="1" min="2" max="27" width="7.0"/>
+    <col min="1" max="1" width="7.43" customWidth="1"/>
+    <col min="2" max="27" width="7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -299,7 +315,7 @@
         <v>26</v>
       </c>
       <c r="B2" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="AA2" s="1" t="s">
         <v>27</v>
@@ -310,22 +326,22 @@
         <v>28</v>
       </c>
       <c r="B3" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G3" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="I3" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="L3" s="1">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="X3" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="Y3" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4">
@@ -333,7 +349,7 @@
         <v>29</v>
       </c>
       <c r="B4" s="1">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>27</v>
@@ -356,13 +372,13 @@
         <v>30</v>
       </c>
       <c r="H5" s="1">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="I5" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="K5" s="1">
-        <v>8.0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6">
@@ -370,16 +386,16 @@
         <v>31</v>
       </c>
       <c r="H6" s="1">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="I6" s="1">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="J6" s="1">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="K6" s="1">
-        <v>10.0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7">
@@ -396,7 +412,7 @@
         <v>27</v>
       </c>
       <c r="L7" s="1">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="X7" s="2" t="s">
         <v>27</v>
@@ -413,7 +429,7 @@
         <v>27</v>
       </c>
       <c r="I8" s="1">
-        <v>13.0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9">
@@ -424,10 +440,10 @@
         <v>27</v>
       </c>
       <c r="I9" s="1">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="Z9" s="1">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="AA9" s="1"/>
     </row>
@@ -439,22 +455,22 @@
         <v>27</v>
       </c>
       <c r="M10" s="1">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="N10" s="1">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="O10" s="1">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="P10" s="1">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="Q10" s="1">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="R10" s="1">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="Z10" s="2" t="s">
         <v>27</v>
@@ -471,13 +487,13 @@
         <v>27</v>
       </c>
       <c r="I11" s="1">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="X11" s="1">
-        <v>22.0</v>
+        <v>22</v>
       </c>
       <c r="Y11" s="1">
-        <v>22.0</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12">
@@ -491,13 +507,13 @@
         <v>27</v>
       </c>
       <c r="J12" s="1">
-        <v>23.0</v>
+        <v>23</v>
       </c>
       <c r="X12" s="1">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="Y12" s="1">
-        <v>24.0</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13">
@@ -511,10 +527,13 @@
         <v>27</v>
       </c>
       <c r="I13" s="1">
-        <v>25.0</v>
+        <v>25</v>
+      </c>
+      <c r="K13" s="0" t="s">
+        <v>27</v>
       </c>
       <c r="Z13" s="1">
-        <v>25.0</v>
+        <v>25</v>
       </c>
       <c r="AA13" s="1"/>
     </row>
@@ -522,32 +541,32 @@
       <c r="A14" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="2">
         <v>27</v>
       </c>
       <c r="H14" s="1">
-        <v>27.0</v>
+        <v>27</v>
       </c>
       <c r="I14" s="1">
-        <v>27.0</v>
+        <v>27</v>
       </c>
       <c r="K14" s="1">
-        <v>27.0</v>
+        <v>27</v>
       </c>
       <c r="S14" s="1">
-        <v>26.0</v>
+        <v>26</v>
       </c>
       <c r="T14" s="1">
-        <v>26.0</v>
+        <v>26</v>
       </c>
       <c r="U14" s="1">
-        <v>26.0</v>
+        <v>26</v>
       </c>
       <c r="V14" s="1">
-        <v>26.0</v>
+        <v>26</v>
       </c>
       <c r="W14" s="1">
-        <v>26.0</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15">
@@ -558,19 +577,19 @@
         <v>27</v>
       </c>
       <c r="S15" s="1">
-        <v>28.0</v>
+        <v>28</v>
       </c>
       <c r="T15" s="1">
-        <v>29.0</v>
+        <v>29</v>
       </c>
       <c r="U15" s="1">
-        <v>31.0</v>
+        <v>31</v>
       </c>
       <c r="V15" s="1">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="W15" s="1">
-        <v>32.0</v>
+        <v>32</v>
       </c>
       <c r="Z15" s="2" t="s">
         <v>27</v>
@@ -590,10 +609,10 @@
         <v>27</v>
       </c>
       <c r="X16" s="1">
-        <v>33.0</v>
+        <v>33</v>
       </c>
       <c r="Y16" s="1">
-        <v>34.0</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17">
@@ -607,7 +626,7 @@
         <v>27</v>
       </c>
       <c r="I17" s="1">
-        <v>35.0</v>
+        <v>35</v>
       </c>
       <c r="M17" s="2" t="s">
         <v>27</v>
@@ -643,7 +662,7 @@
         <v>27</v>
       </c>
       <c r="Z17" s="1">
-        <v>36.0</v>
+        <v>36</v>
       </c>
       <c r="AA17" s="1"/>
     </row>

</xml_diff>